<commit_message>
Fixed SQLite database and excel creation
</commit_message>
<xml_diff>
--- a/ProductTaxes.xlsx
+++ b/ProductTaxes.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Vendor</t>
   </si>
@@ -29,34 +29,13 @@
     <t>Financial Result</t>
   </si>
   <si>
-    <t>Nestle Sofia Corp.</t>
-  </si>
-  <si>
     <t>Zagorka Corp.</t>
   </si>
   <si>
     <t>Targovishte Bottling Company Ltd.</t>
   </si>
   <si>
-    <t>Bella Bulgaria AD</t>
-  </si>
-  <si>
-    <t>Victory OOD</t>
-  </si>
-  <si>
-    <t>Coca Cola Corp.</t>
-  </si>
-  <si>
-    <t>Heineken International</t>
-  </si>
-  <si>
-    <t>Carlsberg International</t>
-  </si>
-  <si>
-    <t>Alpina Distribution</t>
-  </si>
-  <si>
-    <t>Aladin OOD</t>
+    <t>Nestle Sofia Corp.</t>
   </si>
 </sst>
 </file>
@@ -89,7 +68,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,14 +76,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf fontId="0" applyFont="1" xfId="0"/>
-    <xf fontId="1" applyFont="1" fillId="2" applyFill="1" xfId="0"/>
+    <xf fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
     <xf numFmtId="2" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
+    <xf fontId="0" applyFont="1" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="2" applyNumberFormat="1" fontId="0" applyFont="1" borderId="1" applyBorder="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -117,7 +105,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" view="pageLayout"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -146,174 +134,100 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
+        <v>821.8599999999999</v>
+      </c>
+      <c r="C2" s="4">
+        <v>300</v>
+      </c>
+      <c r="D2" s="4">
+        <v>164.37199999999999</v>
+      </c>
+      <c r="E2" s="4">
+        <f>B2-C2-D2</f>
+        <v>357.48799999999994</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1088.6399999999999</v>
+      </c>
+      <c r="C3" s="4">
+        <v>380</v>
+      </c>
+      <c r="D3" s="4">
+        <v>217.72799999999995</v>
+      </c>
+      <c r="E3" s="4">
+        <f>B3-C3-D3</f>
+        <v>490.91199999999992</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
         <v>131.6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C4" s="4">
         <v>70</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D4" s="4">
         <v>26.32</v>
       </c>
-      <c r="E2" s="2">
-        <f>B2-C2-D2</f>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2">
-        <v>821.8599999999999</v>
-      </c>
-      <c r="C3" s="2">
-        <v>300</v>
-      </c>
-      <c r="D3" s="2">
-        <v>164.37199999999999</v>
-      </c>
-      <c r="E3" s="2">
-        <f>B3-C3-D3</f>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1088.6399999999999</v>
-      </c>
-      <c r="C4" s="2">
-        <v>380</v>
-      </c>
-      <c r="D4" s="2">
-        <v>217.72799999999995</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <f>B4-C4-D4</f>
+        <v>35.279999999999994</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <f>B5-C5-D5</f>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <f>B6-C6-D6</f>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <f>B7-C7-D7</f>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <f>B8-C8-D8</f>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <f>B9-C9-D9</f>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <f>B10-C10-D10</f>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <f>B11-C11-D11</f>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12">
       <c r="B12" s="2"/>
@@ -850,6 +764,8 @@
       <c r="E100" s="2"/>
     </row>
   </sheetData>
-  <headerFooter/>
+  <headerFooter differentFirst="1">
+    <firstHeader>&amp;CБаси данъците чуек</firstHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>